<commit_message>
finished scraper last touches to be added
</commit_message>
<xml_diff>
--- a/src/scraping-fmcsa.dot.gov/carriers.xlsx
+++ b/src/scraping-fmcsa.dot.gov/carriers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="199">
   <si>
     <t>usdot_number</t>
   </si>
@@ -32,6 +32,582 @@
   </si>
   <si>
     <t>state</t>
+  </si>
+  <si>
+    <t>1128010</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>459929</t>
+  </si>
+  <si>
+    <t>COLUMBIA INTERMODAL LLC</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>LIBERTY CORNER</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>4098535</t>
+  </si>
+  <si>
+    <t>1572948</t>
+  </si>
+  <si>
+    <t>HERE2THERE LOGISTICAL TRANSPORT LLC</t>
+  </si>
+  <si>
+    <t>EAST ORANGE</t>
+  </si>
+  <si>
+    <t>2891880</t>
+  </si>
+  <si>
+    <t>972556</t>
+  </si>
+  <si>
+    <t>LHT LLC</t>
+  </si>
+  <si>
+    <t>BUDD LAKE</t>
+  </si>
+  <si>
+    <t>2842554</t>
+  </si>
+  <si>
+    <t>953989</t>
+  </si>
+  <si>
+    <t>PAC TRANSPORTATION &amp; LOGISTICS LLC</t>
+  </si>
+  <si>
+    <t>CLEMENTON</t>
+  </si>
+  <si>
+    <t>3597092</t>
+  </si>
+  <si>
+    <t>1254552</t>
+  </si>
+  <si>
+    <t>SB INTERSATE LLC</t>
+  </si>
+  <si>
+    <t>CRANFORD</t>
+  </si>
+  <si>
+    <t>4193136</t>
+  </si>
+  <si>
+    <t>1632876</t>
+  </si>
+  <si>
+    <t>STEVEN TRANSPORT SERVICES LLC</t>
+  </si>
+  <si>
+    <t>IRVINGTON</t>
+  </si>
+  <si>
+    <t>4126531</t>
+  </si>
+  <si>
+    <t>1633454</t>
+  </si>
+  <si>
+    <t>THECH LOGISTICS LLC</t>
+  </si>
+  <si>
+    <t>THECH LOGISTICS</t>
+  </si>
+  <si>
+    <t>WILLINGBORO</t>
+  </si>
+  <si>
+    <t>4199871</t>
+  </si>
+  <si>
+    <t>1632405</t>
+  </si>
+  <si>
+    <t>TRIPLE C TRUCKING LLC</t>
+  </si>
+  <si>
+    <t>MOUNT HOLLY</t>
+  </si>
+  <si>
+    <t>157652</t>
+  </si>
+  <si>
+    <t>144502</t>
+  </si>
+  <si>
+    <t>"ATKINSON-INTERMODAL SYSTEMS, INC. "</t>
+  </si>
+  <si>
+    <t>JERSEY CITY</t>
+  </si>
+  <si>
+    <t>511774</t>
+  </si>
+  <si>
+    <t>234067</t>
+  </si>
+  <si>
+    <t>"BEDA"INTERSTATE TRANSIT, INC.</t>
+  </si>
+  <si>
+    <t>UNION CITY</t>
+  </si>
+  <si>
+    <t>611184</t>
+  </si>
+  <si>
+    <t>297297</t>
+  </si>
+  <si>
+    <t>"HEARD YOU'RE MOVING," CO.</t>
+  </si>
+  <si>
+    <t>SOMERSET</t>
+  </si>
+  <si>
+    <t>180841</t>
+  </si>
+  <si>
+    <t>"TAC II, INC. "</t>
+  </si>
+  <si>
+    <t>TRENTON</t>
+  </si>
+  <si>
+    <t>1252058</t>
+  </si>
+  <si>
+    <t>494081</t>
+  </si>
+  <si>
+    <t>"WALDO" TRUCKING CORP.</t>
+  </si>
+  <si>
+    <t>PAULSBORO</t>
+  </si>
+  <si>
+    <t>4091974</t>
+  </si>
+  <si>
+    <t>1576634</t>
+  </si>
+  <si>
+    <t>0202 TRANSPORTATION CORP</t>
+  </si>
+  <si>
+    <t>RIDGEFIELD</t>
+  </si>
+  <si>
+    <t>3158523</t>
+  </si>
+  <si>
+    <t>109503</t>
+  </si>
+  <si>
+    <t>07 ZERO STONE LLC</t>
+  </si>
+  <si>
+    <t>HIGHTSTOWN</t>
+  </si>
+  <si>
+    <t>2953329</t>
+  </si>
+  <si>
+    <t>377</t>
+  </si>
+  <si>
+    <t>1 &amp; 1 LOGISTICS INC</t>
+  </si>
+  <si>
+    <t>COLTS NECK</t>
+  </si>
+  <si>
+    <t>3805727</t>
+  </si>
+  <si>
+    <t>1371503</t>
+  </si>
+  <si>
+    <t>1 &amp; 9 LLC</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>1641110</t>
+  </si>
+  <si>
+    <t>726366</t>
+  </si>
+  <si>
+    <t>1 A WAY TRUCKING LLC</t>
+  </si>
+  <si>
+    <t>NORTH ARLINGTON</t>
+  </si>
+  <si>
+    <t>3786790</t>
+  </si>
+  <si>
+    <t>1357683</t>
+  </si>
+  <si>
+    <t>1 APLUS LOGISTICS LLC</t>
+  </si>
+  <si>
+    <t>NEWARK</t>
+  </si>
+  <si>
+    <t>2919323</t>
+  </si>
+  <si>
+    <t>984548</t>
+  </si>
+  <si>
+    <t>1 CITY WIDE TRANSPORTATION LLC</t>
+  </si>
+  <si>
+    <t>CALDWELL</t>
+  </si>
+  <si>
+    <t>2195871</t>
+  </si>
+  <si>
+    <t>842083</t>
+  </si>
+  <si>
+    <t>1 EXTREME TOWING CORP</t>
+  </si>
+  <si>
+    <t>3344773</t>
+  </si>
+  <si>
+    <t>1068219</t>
+  </si>
+  <si>
+    <t>1 FREEDOM TRUCKING LLC</t>
+  </si>
+  <si>
+    <t>PLAINFIELD</t>
+  </si>
+  <si>
+    <t>2608212</t>
+  </si>
+  <si>
+    <t>912942</t>
+  </si>
+  <si>
+    <t>1 NATION TRANSPORTATION LLC</t>
+  </si>
+  <si>
+    <t>CLIFTON</t>
+  </si>
+  <si>
+    <t>3983044</t>
+  </si>
+  <si>
+    <t>1511620</t>
+  </si>
+  <si>
+    <t>1 OAK TRANSPORT</t>
+  </si>
+  <si>
+    <t>N BRUNSWICK</t>
+  </si>
+  <si>
+    <t>3250237</t>
+  </si>
+  <si>
+    <t>1022718</t>
+  </si>
+  <si>
+    <t>1 ONKAR TRANSPORT INC</t>
+  </si>
+  <si>
+    <t>VOORHEES</t>
+  </si>
+  <si>
+    <t>913340</t>
+  </si>
+  <si>
+    <t>394978</t>
+  </si>
+  <si>
+    <t>1 RATE MOVING, INC.</t>
+  </si>
+  <si>
+    <t>TEANECK</t>
+  </si>
+  <si>
+    <t>1953508</t>
+  </si>
+  <si>
+    <t>767606</t>
+  </si>
+  <si>
+    <t>1 RELIABLE TRANSPORTATION INC</t>
+  </si>
+  <si>
+    <t>HACKENSACK</t>
+  </si>
+  <si>
+    <t>2064936</t>
+  </si>
+  <si>
+    <t>727865</t>
+  </si>
+  <si>
+    <t>1 SOURCE LOGISTICS LLC</t>
+  </si>
+  <si>
+    <t>NORTH BERGEN</t>
+  </si>
+  <si>
+    <t>1618672</t>
+  </si>
+  <si>
+    <t>598065</t>
+  </si>
+  <si>
+    <t>1 ST MOVING CORP</t>
+  </si>
+  <si>
+    <t>HOWELL</t>
+  </si>
+  <si>
+    <t>2446041</t>
+  </si>
+  <si>
+    <t>844079</t>
+  </si>
+  <si>
+    <t>1 STOP TOWING AND RECOVERY LLC</t>
+  </si>
+  <si>
+    <t>1 STOP TOWING AND RECOVERY</t>
+  </si>
+  <si>
+    <t>CAMDEN</t>
+  </si>
+  <si>
+    <t>1033969</t>
+  </si>
+  <si>
+    <t>1 TRADE EXPRESS LLC</t>
+  </si>
+  <si>
+    <t>PERTH AMBOY</t>
+  </si>
+  <si>
+    <t>2050107</t>
+  </si>
+  <si>
+    <t>718229</t>
+  </si>
+  <si>
+    <t>1 USA CARRIERS INC</t>
+  </si>
+  <si>
+    <t>EAST BRUNSWICK</t>
+  </si>
+  <si>
+    <t>3945100</t>
+  </si>
+  <si>
+    <t>1466362</t>
+  </si>
+  <si>
+    <t>1 WAY LOGISTICS LLC</t>
+  </si>
+  <si>
+    <t>PASSAIC</t>
+  </si>
+  <si>
+    <t>3552657</t>
+  </si>
+  <si>
+    <t>1190382</t>
+  </si>
+  <si>
+    <t>1 WORKING MOM LLC</t>
+  </si>
+  <si>
+    <t>2349080</t>
+  </si>
+  <si>
+    <t>804026</t>
+  </si>
+  <si>
+    <t>1&amp;1 TRANSPORTATION INC</t>
+  </si>
+  <si>
+    <t>BAYONNE</t>
+  </si>
+  <si>
+    <t>17445</t>
+  </si>
+  <si>
+    <t>1-844-SIR-JUNK LLC</t>
+  </si>
+  <si>
+    <t>RAMSEY</t>
+  </si>
+  <si>
+    <t>4198134</t>
+  </si>
+  <si>
+    <t>1619004</t>
+  </si>
+  <si>
+    <t>1-OAK INVESTMENTS  LLC</t>
+  </si>
+  <si>
+    <t>1-OAK</t>
+  </si>
+  <si>
+    <t>HAMMONTON</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>54216</t>
+  </si>
+  <si>
+    <t>100PERCENTSOLUTIONSLLC</t>
+  </si>
+  <si>
+    <t>3870795</t>
+  </si>
+  <si>
+    <t>1430228</t>
+  </si>
+  <si>
+    <t>3745117</t>
+  </si>
+  <si>
+    <t>1327235</t>
+  </si>
+  <si>
+    <t>101 EXPRESS CORPORATION</t>
+  </si>
+  <si>
+    <t>4024556</t>
+  </si>
+  <si>
+    <t>1518889</t>
+  </si>
+  <si>
+    <t>101 MOVERS CORP</t>
+  </si>
+  <si>
+    <t>4035015</t>
+  </si>
+  <si>
+    <t>1525472</t>
+  </si>
+  <si>
+    <t>101 TRUCKING CORPORATION</t>
+  </si>
+  <si>
+    <t>3679375</t>
+  </si>
+  <si>
+    <t>1279064</t>
+  </si>
+  <si>
+    <t>1019 TRUCKING LLC</t>
+  </si>
+  <si>
+    <t>1019 TRUCKING</t>
+  </si>
+  <si>
+    <t>PATERSON</t>
+  </si>
+  <si>
+    <t>3204211</t>
+  </si>
+  <si>
+    <t>197535</t>
+  </si>
+  <si>
+    <t>1023 HUDSON AVE DESSERTS LLC</t>
+  </si>
+  <si>
+    <t>MR TODS PIES</t>
+  </si>
+  <si>
+    <t>5769</t>
+  </si>
+  <si>
+    <t>12 STAR LEASING CORP.</t>
+  </si>
+  <si>
+    <t>WARREN</t>
+  </si>
+  <si>
+    <t>4091968</t>
+  </si>
+  <si>
+    <t>1559057</t>
+  </si>
+  <si>
+    <t>1209 INDUSTRIES LLC</t>
+  </si>
+  <si>
+    <t>PARAMUS</t>
+  </si>
+  <si>
+    <t>3895802OOS</t>
+  </si>
+  <si>
+    <t>1433691</t>
+  </si>
+  <si>
+    <t>122 VAN GUARD LLC</t>
+  </si>
+  <si>
+    <t>3379230</t>
+  </si>
+  <si>
+    <t>1084320</t>
+  </si>
+  <si>
+    <t>123 LIMO &amp; CAR SERVICE LLC</t>
+  </si>
+  <si>
+    <t>2951246</t>
+  </si>
+  <si>
+    <t>999289</t>
+  </si>
+  <si>
+    <t>123 TOWING INC</t>
+  </si>
+  <si>
+    <t>3158285</t>
+  </si>
+  <si>
+    <t>109342</t>
+  </si>
+  <si>
+    <t>123 TRANSPORT USA INC</t>
+  </si>
+  <si>
+    <t>KENILWORTH</t>
   </si>
 </sst>
 </file>
@@ -408,7 +984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G51"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -434,6 +1010,1156 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38" t="s">
+        <v>155</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>176</v>
+      </c>
+      <c r="D45" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F45" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>185</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>187</v>
+      </c>
+      <c r="D48" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>189</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>192</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" t="s">
+        <v>194</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>198</v>
+      </c>
+      <c r="G51" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>